<commit_message>
Finalize scenario properties excel documentation file
</commit_message>
<xml_diff>
--- a/doc/ScenarioProperties.xlsx
+++ b/doc/ScenarioProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SPOT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA292E0-9089-40CC-85E8-EB227726EB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1399EEB4-C2C6-4CDF-B627-BFDE3AEB4EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{3F79704C-5C77-497F-8298-D98309975613}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -216,6 +216,140 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>false</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Valid file path
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(always use '/' for path separator)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>debug_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;yyyyMMddHHmmss&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.log</t>
+    </r>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Properties files location</t>
+  </si>
+  <si>
+    <t>Timeouts</t>
+  </si>
+  <si>
+    <t>timeout</t>
+  </si>
+  <si>
+    <t>Any positive value</t>
+  </si>
+  <si>
+    <t>timeoutShort</t>
+  </si>
+  <si>
+    <t>timeoutToOpenPage</t>
+  </si>
+  <si>
+    <t>Expressed in seconds, which is used by default when waiting for any kind of operation (typically getting a web element in the page).</t>
+  </si>
+  <si>
+    <t>Expressed in seconds, which is used by default when waiting for short operation (typically get web elements inside an already found web element).</t>
+  </si>
+  <si>
+    <t>Expressed in seconds, which is used to wait for a page or any main web element (dialog, menu, etc.) in a page to be opened at a first time.</t>
+  </si>
+  <si>
+    <t>Global timeout value for short operations</t>
+  </si>
+  <si>
+    <t>Global timeout value for opening operations</t>
+  </si>
+  <si>
+    <t>Global timeout value for any operation</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Each file path must be relative to the </t>
     </r>
@@ -223,21 +357,11 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>nestedP</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
         <color theme="4" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>aramFilesDir</t>
+      <t>nestedParamFilesDir</t>
     </r>
     <r>
       <rPr>
@@ -260,145 +384,1118 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>false</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Valid file path
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(always use '/' for path separator)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>debug_</t>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>browserKind</t>
+  </si>
+  <si>
+    <t>The kind of browser use to run the scenario.</t>
+  </si>
+  <si>
+    <t>browserPath</t>
+  </si>
+  <si>
+    <t>The path to find the browser executable.</t>
+  </si>
+  <si>
+    <t>If not specified, the browser is supposed to be on your system path.</t>
+  </si>
+  <si>
+    <t>browserProfile</t>
+  </si>
+  <si>
+    <t>The path for the profile to be used.</t>
+  </si>
+  <si>
+    <t>If not specified, the default browser profile is used.</t>
+  </si>
+  <si>
+    <t>windowSize</t>
+  </si>
+  <si>
+    <t>Specify the size of the window when opening the browser.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any string formatted as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>"</t>
     </r>
     <r>
       <rPr>
         <i/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;yyyyMMddHHmmss&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.log</t>
-    </r>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>Properties files location</t>
-  </si>
-  <si>
-    <t>Timeouts</t>
-  </si>
-  <si>
-    <t>timeout</t>
-  </si>
-  <si>
-    <t>Any positive value</t>
-  </si>
-  <si>
-    <t>timeoutShort</t>
-  </si>
-  <si>
-    <t>timeoutToOpenPage</t>
-  </si>
-  <si>
-    <t>Expressed in seconds, which is used by default when waiting for any kind of operation (typically getting a web element in the page).</t>
-  </si>
-  <si>
-    <t>Expressed in seconds, which is used by default when waiting for short operation (typically get web elements inside an already found web element).</t>
-  </si>
-  <si>
-    <t>Expressed in seconds, which is used to wait for a page or any main web element (dialog, menu, etc.) in a page to be opened at a first time.</t>
-  </si>
-  <si>
-    <t>Global timeout value for short operations</t>
-  </si>
-  <si>
-    <t>Global timeout value for opening operations</t>
-  </si>
-  <si>
-    <t>Global timeout value for any operation</t>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>&lt;height&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>&lt;width&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>"900x1600"</t>
+  </si>
+  <si>
+    <t>selenium.snapshots.dir</t>
+  </si>
+  <si>
+    <t>The directory path were snapshots (info, warning and error) will be put during the scenario execution.</t>
+  </si>
+  <si>
+    <t>snapshots</t>
+  </si>
+  <si>
+    <t>Can be a relative path (as for default value). In this case the root is the scenario project directory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Firefox)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Internet Explorer)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Google Chrome), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (MS Edge), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Safari)</t>
+    </r>
+  </si>
+  <si>
+    <t>Height value as to be between 900 and 1200,
+Width value has to be between 1200 and 1920.</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>firstStep</t>
+  </si>
+  <si>
+    <t>Complete or part of scenario step name</t>
+  </si>
+  <si>
+    <t>lastStep</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>List of strings separated by comma (without spaces). Each string is a complete or a part of scenario step name</t>
+  </si>
+  <si>
+    <t>firstTest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Complete or part of test name of the scenario </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>first step</t>
+    </r>
+  </si>
+  <si>
+    <t>lastTest</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>List of tests to run for the first executed step.</t>
+  </si>
+  <si>
+    <t>stopOnFailure</t>
+  </si>
+  <si>
+    <t>Flag telling the scenario to stop as soon as a test failure occurs.</t>
+  </si>
+  <si>
+    <t>stopOnException</t>
+  </si>
+  <si>
+    <t>Flag telling the scenario to stop as soon as an exception occurs in a test.</t>
+  </si>
+  <si>
+    <t>Step from which the scenario run will start</t>
+  </si>
+  <si>
+    <t>Step at which the scenario run will finish</t>
+  </si>
+  <si>
+    <t>List of steps to run</t>
+  </si>
+  <si>
+    <t>First step test from which the scenario run will start</t>
+  </si>
+  <si>
+    <t>Complete or part of test name of the scenario first step</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If this argument is set, the scenario will ignore all steps in its list until it finds one containing the given value.
+Example of VM arguments used for Sample Tools QA scenario:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-DfirstStep=01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: scenario execution starts from step </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep01_Dialog</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If this argument is set, the scenario will ignore all steps in its list after having found one containing the given value.
+Example of VM arguments used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sample Tools QA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> scenario:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-DlastStep=01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: Scenario execution ends at step </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep00_TextBox</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This argument overrides </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>firstStep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>lastStep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> arguments values if they are also defined.
+Note that this argument allow several non-contiguous steps to be run in one shot.
+If this argument is set, the scenario will execute only the steps given in the given list value.
+Examples of VM arguments used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sample Tools QA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> scenario:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-Dsteps=01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: only step </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep01_Dialog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is executed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-Dsteps=00,01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: both steps </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep00_TextBox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep01_Dialog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> are executed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If this argument is set, the scenario will ignore all first step tests until it finds one containing the given value.
+Examples of VM arguments used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sample Tools QA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> scenario:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-DfirstSteps=01 -DfirstTest=02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: scenario execution start from test </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>test02_LargeModal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of step </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep01_Dialog</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If this argument is set, the scenario will ignore all last step tests after having found the test containing the given value.
+Examples of VM arguments used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sample Tools QA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> scenario:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-DlastSteps=00 -DlastTest=02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: scenario execution ends at test </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>test02_Email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of step </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep00_TextBox</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List of strings separated by comma (without spaces). Each string is a complete or part of test name of the scenario </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>first step</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This argument overrides </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>firstTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>lastTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> arguments values if they are also defined.
+Note that this argument allow several non-contiguous tests to be run in one shot.
+If this argument is set, the scenario will execute only the tests given in the given list value.
+Examples of VM arguments used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sample Tools QA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> scenario:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-Dsteps=01 -Dtests=01,03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: only tests </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>test01_FullName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>test03_CurrentAddress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of step </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep01_Dialog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> are executed</t>
+    </r>
+  </si>
+  <si>
+    <t>data.creation.behavior</t>
+  </si>
+  <si>
+    <t>Possible strategies while encountering existing data during creation operation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>error, reuse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When set to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, the scenario is supposed to fail if existing data it tries to create already exists on the server. When set to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>reuse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, the scenario is supposed to skip the creation operation and reuse the existing data. When set to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, the scenario is supposed to first delete the existing data, then perform the creation operation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>duplicationMode</t>
+  </si>
+  <si>
+    <t>Defined the way the framework handle duplicated properties definition</t>
+  </si>
+  <si>
+    <t>forbidden</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>overwrite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ignore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>forbidden</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Framework behavior is defined as follows when duplicated property definition is encountered:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>overwrite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: last read definition is used
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ignore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: first read definition is used
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>forbidden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: a ScenarioFailedError is raised</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,6 +1575,52 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -560,10 +1703,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -572,19 +1718,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -598,29 +1735,69 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Code" xfId="1" xr:uid="{7A515A9B-B31A-446B-BE42-56C71C9280CB}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -933,28 +2110,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EFC48D-9583-484F-B028-08D0FE7425F8}">
-  <dimension ref="A2:E24"/>
+  <dimension ref="A2:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="3" width="40.7109375" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="120.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="27" thickBot="1">
-      <c r="A2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
       <c r="A3" s="2" t="s">
@@ -974,41 +2151,41 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" thickTop="1" thickBot="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" thickTop="1" thickBot="1">
+      <c r="A5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" thickTop="1" thickBot="1">
-      <c r="A5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1017,46 +2194,46 @@
       <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>36</v>
+      <c r="D6" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" thickTop="1" thickBot="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickTop="1"/>
     <row r="10" spans="1:5" ht="27" thickBot="1">
-      <c r="A10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
       <c r="A11" s="2" t="s">
@@ -1085,7 +2262,7 @@
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1093,19 +2270,19 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1119,7 +2296,7 @@
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1127,115 +2304,432 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickTop="1"/>
-    <row r="18" spans="1:5" ht="27" thickBot="1">
-      <c r="A18" s="9" t="s">
+      <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60.75" thickTop="1" thickBot="1">
+      <c r="A16" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickTop="1"/>
+    <row r="19" spans="1:5" ht="27" thickBot="1">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" thickTop="1" thickBot="1">
+      <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
-      <c r="A19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" thickTop="1" thickBot="1">
-      <c r="A20" s="15" t="s">
+      <c r="B21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="17">
+      <c r="D21" s="23">
         <v>60</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" thickTop="1" thickBot="1">
-      <c r="A21" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="20">
-        <v>10</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>45</v>
+      <c r="E21" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" thickTop="1" thickBot="1">
       <c r="A22" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="17">
+      <c r="B22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="24">
+        <v>10</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" thickTop="1" thickBot="1">
+      <c r="A23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="23">
         <v>20</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickTop="1"/>
+      <c r="E23" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickTop="1"/>
+    <row r="26" spans="1:5" ht="27" thickBot="1">
+      <c r="A26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+      <c r="A27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" thickTop="1" thickBot="1">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="25">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="30" thickTop="1" thickBot="1">
+      <c r="A29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" thickTop="1" thickBot="1">
+      <c r="A30" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A31" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickTop="1"/>
+    <row r="35" spans="1:5" ht="27" thickBot="1">
+      <c r="A35" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="59.25" thickTop="1" thickBot="1">
+      <c r="A37" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="66.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A38" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A39" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A40" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="73.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A41" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="104.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A44" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A46" s="13"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tune scenario properties Excel doc file
</commit_message>
<xml_diff>
--- a/doc/ScenarioProperties.xlsx
+++ b/doc/ScenarioProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SPOT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1399EEB4-C2C6-4CDF-B627-BFDE3AEB4EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD92D10-4B1D-4277-8897-1407A7B97FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{3F79704C-5C77-497F-8298-D98309975613}"/>
   </bookViews>
@@ -2112,8 +2112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EFC48D-9583-484F-B028-08D0FE7425F8}">
   <dimension ref="A2:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix wrong format in scenario properties Excel doc file
</commit_message>
<xml_diff>
--- a/doc/ScenarioProperties.xlsx
+++ b/doc/ScenarioProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SPOT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD92D10-4B1D-4277-8897-1407A7B97FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C8FA3D-B45F-425B-BA2B-7ADADBB88FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{3F79704C-5C77-497F-8298-D98309975613}"/>
   </bookViews>
@@ -1495,7 +1495,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1612,12 +1612,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1709,7 +1703,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1783,13 +1777,10 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2330,7 +2321,7 @@
       <c r="C16" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="29" t="s">
         <v>104</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -2515,7 +2506,7 @@
       <c r="C31" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="27" t="s">
         <v>62</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -2532,7 +2523,7 @@
       <c r="C32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="28" t="s">
         <v>65</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -2668,7 +2659,7 @@
       <c r="C42" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="5" t="s">

</xml_diff>

<commit_message>
Update Scenario Properties documentation file
</commit_message>
<xml_diff>
--- a/doc/ScenarioProperties.xlsx
+++ b/doc/ScenarioProperties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SPOT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C8FA3D-B45F-425B-BA2B-7ADADBB88FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F2E939-2CDD-4F1A-BCA5-A18074DFC909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{3F79704C-5C77-497F-8298-D98309975613}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -284,30 +284,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>debug_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;yyyyMMddHHmmss&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.log</t>
     </r>
   </si>
   <si>
@@ -1488,6 +1464,191 @@
         <family val="2"/>
       </rPr>
       <t>: a ScenarioFailedError is raised</t>
+    </r>
+  </si>
+  <si>
+    <t>failuresThreshold</t>
+  </si>
+  <si>
+    <t>Threshold for failures occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <t>When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it</t>
+  </si>
+  <si>
+    <r>
+      <t>debug_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;timestamp&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.log</t>
+    </r>
+  </si>
+  <si>
+    <t>Threshold for retryable errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A retryable error is any error subclass of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>RetryableError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>retriablesThreshold</t>
+  </si>
+  <si>
+    <t>alertsThreshold</t>
+  </si>
+  <si>
+    <t>Threshold for alert errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <t>multiplesThreshold</t>
+  </si>
+  <si>
+    <t>browserErrorsThreshold</t>
+  </si>
+  <si>
+    <t>Threshold for multiple errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <t>Threshold for browser errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. An alert error is an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>UnhandledAlertException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A browser error is either a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>UnreachableBrowserException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, a kind of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>BrowserError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>WebDriverException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> with some specific browser related message.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A multiple error is a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>MultipleVisibleElementsError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -1495,7 +1656,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1562,13 +1723,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color theme="1"/>
@@ -1615,6 +1769,18 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1703,7 +1869,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1718,7 +1884,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1771,19 +1937,22 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2101,23 +2270,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EFC48D-9583-484F-B028-08D0FE7425F8}">
-  <dimension ref="A2:E47"/>
+  <dimension ref="A2:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="120.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="113.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="27" thickBot="1">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2185,8 +2354,8 @@
       <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>35</v>
+      <c r="D6" s="30" t="s">
+        <v>109</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
@@ -2219,7 +2388,7 @@
     <row r="9" spans="1:5" ht="15.75" thickTop="1"/>
     <row r="10" spans="1:5" ht="27" thickBot="1">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2308,24 +2477,24 @@
         <v>8</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="60.75" thickTop="1" thickBot="1">
       <c r="A16" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
@@ -2338,7 +2507,7 @@
     <row r="18" spans="1:5" ht="15.75" thickTop="1"/>
     <row r="19" spans="1:5" ht="27" thickBot="1">
       <c r="A19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2364,53 +2533,53 @@
     </row>
     <row r="21" spans="1:5" ht="30" thickTop="1" thickBot="1">
       <c r="A21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="D21" s="23">
         <v>60</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" thickTop="1" thickBot="1">
       <c r="A22" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="24">
         <v>10</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" thickTop="1" thickBot="1">
       <c r="A23" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="23">
         <v>20</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
@@ -2423,7 +2592,7 @@
     <row r="25" spans="1:5" ht="15.75" thickTop="1"/>
     <row r="26" spans="1:5" ht="27" thickBot="1">
       <c r="A26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2449,13 +2618,13 @@
     </row>
     <row r="28" spans="1:5" ht="30" thickTop="1" thickBot="1">
       <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="25">
         <v>1</v>
@@ -2464,10 +2633,10 @@
     </row>
     <row r="29" spans="1:5" ht="30" thickTop="1" thickBot="1">
       <c r="A29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>7</v>
@@ -2476,15 +2645,15 @@
         <v>8</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" thickTop="1" thickBot="1">
       <c r="A30" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>7</v>
@@ -2493,41 +2662,41 @@
         <v>8</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A31" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="27" t="s">
-        <v>62</v>
-      </c>
       <c r="E31" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1">
       <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
@@ -2540,7 +2709,7 @@
     <row r="34" spans="1:5" ht="15.75" thickTop="1"/>
     <row r="35" spans="1:5" ht="27" thickBot="1">
       <c r="A35" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2566,161 +2735,246 @@
     </row>
     <row r="37" spans="1:5" ht="59.25" thickTop="1" thickBot="1">
       <c r="A37" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="66.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="66.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="17" t="s">
+    <row r="39" spans="1:5" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A39" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="16" t="s">
+      <c r="C39" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A40" s="17" t="s">
+    <row r="41" spans="1:5" ht="73.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A41" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="73.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A41" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="104.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="C42" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>96</v>
+      <c r="E42" s="10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="3"/>
+      <c r="D43" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A44" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="25">
+        <v>2</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A45" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="29">
+        <v>5</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30.75" thickTop="1" thickBot="1">
+      <c r="A46" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="25">
+        <v>10</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30.75" thickTop="1" thickBot="1">
+      <c r="A47" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="29">
+        <v>2</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45" thickTop="1" thickBot="1">
+      <c r="A48" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="25">
+        <v>2</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30" thickTop="1" thickBot="1">
+      <c r="A49" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A45" s="1" t="s">
+      <c r="D49" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5" ht="45.75" thickTop="1" thickBot="1">
+      <c r="A50" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D50" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A46" s="13"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" thickTop="1"/>
+    </row>
+    <row r="51" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A51" s="17"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="7"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update doc for tests parameter
</commit_message>
<xml_diff>
--- a/doc/ScenarioProperties.xlsx
+++ b/doc/ScenarioProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SPOT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F2E939-2CDD-4F1A-BCA5-A18074DFC909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74B0C68-8F78-4050-AC0E-9B729ECEE162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{3F79704C-5C77-497F-8298-D98309975613}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18720" xr2:uid="{3F79704C-5C77-497F-8298-D98309975613}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,9 +654,6 @@
     <t>tests</t>
   </si>
   <si>
-    <t>List of tests to run for the first executed step.</t>
-  </si>
-  <si>
     <t>stopOnFailure</t>
   </si>
   <si>
@@ -1070,19 +1067,440 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">List of strings separated by comma (without spaces). Each string is a complete or part of test name of the scenario </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>first step</t>
-    </r>
+    <t>data.creation.behavior</t>
+  </si>
+  <si>
+    <t>Possible strategies while encountering existing data during creation operation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>error, reuse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When set to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, the scenario is supposed to fail if existing data it tries to create already exists on the server. When set to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>reuse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, the scenario is supposed to skip the creation operation and reuse the existing data. When set to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, the scenario is supposed to first delete the existing data, then perform the creation operation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>duplicationMode</t>
+  </si>
+  <si>
+    <t>Defined the way the framework handle duplicated properties definition</t>
+  </si>
+  <si>
+    <t>forbidden</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>overwrite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ignore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>forbidden</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Framework behavior is defined as follows when duplicated property definition is encountered:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>overwrite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: last read definition is used
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ignore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: first read definition is used
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>forbidden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: a ScenarioFailedError is raised</t>
+    </r>
+  </si>
+  <si>
+    <t>failuresThreshold</t>
+  </si>
+  <si>
+    <t>Threshold for failures occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <t>When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it</t>
+  </si>
+  <si>
+    <r>
+      <t>debug_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;timestamp&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.log</t>
+    </r>
+  </si>
+  <si>
+    <t>Threshold for retryable errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A retryable error is any error subclass of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>RetryableError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>retriablesThreshold</t>
+  </si>
+  <si>
+    <t>alertsThreshold</t>
+  </si>
+  <si>
+    <t>Threshold for alert errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <t>multiplesThreshold</t>
+  </si>
+  <si>
+    <t>browserErrorsThreshold</t>
+  </si>
+  <si>
+    <t>Threshold for multiple errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <t>Threshold for browser errors occurring during the whole scenario execution</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. An alert error is an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>UnhandledAlertException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A browser error is either a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>UnreachableBrowserException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, a kind of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>BrowserError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>WebDriverException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> with some specific browser related message.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A multiple error is a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>MultipleVisibleElementsError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>List of tests to run for the executed steps.</t>
+  </si>
+  <si>
+    <t>List of strings separated by comma (without spaces). Each string is a complete or part of test name for all scenario steps or only for specific step if specified.
+Usage of * is now allowed for this parameter</t>
   </si>
   <si>
     <r>
@@ -1219,436 +1637,99 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> are executed</t>
-    </r>
-  </si>
-  <si>
-    <t>data.creation.behavior</t>
-  </si>
-  <si>
-    <t>Possible strategies while encountering existing data during creation operation</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>error, reuse</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>delete</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When set to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>error</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, the scenario is supposed to fail if existing data it tries to create already exists on the server. When set to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>reuse</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, the scenario is supposed to skip the creation operation and reuse the existing data. When set to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>delete</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, the scenario is supposed to first delete the existing data, then perform the creation operation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>error</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>duplicationMode</t>
-  </si>
-  <si>
-    <t>Defined the way the framework handle duplicated properties definition</t>
-  </si>
-  <si>
-    <t>forbidden</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>overwrite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ignore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>forbidden</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Framework behavior is defined as follows when duplicated property definition is encountered:
+      <t xml:space="preserve"> are executed
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>overwrite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: last read definition is used
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-Dtests=01.01,01.03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: same as above by using specific step in tests parameter syntax
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ignore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: first read definition is used
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>forbidden</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>: a ScenarioFailedError is raised</t>
-    </r>
-  </si>
-  <si>
-    <t>failuresThreshold</t>
-  </si>
-  <si>
-    <t>Threshold for failures occurring during the whole scenario execution</t>
-  </si>
-  <si>
-    <t>When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it</t>
-  </si>
-  <si>
-    <r>
-      <t>debug_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;timestamp&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.log</t>
-    </r>
-  </si>
-  <si>
-    <t>Threshold for retryable errors occurring during the whole scenario execution</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A retryable error is any error subclass of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>RetryableError</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>retriablesThreshold</t>
-  </si>
-  <si>
-    <t>alertsThreshold</t>
-  </si>
-  <si>
-    <t>Threshold for alert errors occurring during the whole scenario execution</t>
-  </si>
-  <si>
-    <t>multiplesThreshold</t>
-  </si>
-  <si>
-    <t>browserErrorsThreshold</t>
-  </si>
-  <si>
-    <t>Threshold for multiple errors occurring during the whole scenario execution</t>
-  </si>
-  <si>
-    <t>Threshold for browser errors occurring during the whole scenario execution</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. An alert error is an </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>UnhandledAlertException</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A browser error is either a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>UnreachableBrowserException</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, a kind of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>BrowserError</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> or a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>WebDriverException</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> with some specific browser related message.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When more than this threshold of errors has occurred since the beginning of the scenario execution, then framework stops it. A multiple error is a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>MultipleVisibleElementsError</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-Dtests=01.*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: run all tests of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SampleToolsQaStep01_Dialog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, this is equivalent to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-Dsteps=01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> but allow addition of other tests if necessary using only the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>tests</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> parameter</t>
     </r>
   </si>
 </sst>
@@ -2272,19 +2353,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EFC48D-9583-484F-B028-08D0FE7425F8}">
   <dimension ref="A2:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="113.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.69140625" customWidth="1"/>
+    <col min="2" max="3" width="40.69140625" customWidth="1"/>
+    <col min="4" max="4" width="23.3828125" customWidth="1"/>
+    <col min="5" max="5" width="113.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="27" thickBot="1">
+    <row r="2" spans="1:5" ht="26.6" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>35</v>
       </c>
@@ -2293,7 +2374,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+    <row r="3" spans="1:5" ht="18.45" thickTop="1" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +2391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="4" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -2327,7 +2408,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="5" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A5" s="13" t="s">
         <v>20</v>
       </c>
@@ -2344,7 +2425,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    <row r="6" spans="1:5" ht="15.45" thickTop="1" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2355,13 +2436,13 @@
         <v>25</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="7" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
@@ -2378,15 +2459,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    <row r="8" spans="1:5" ht="15.45" thickTop="1" thickBot="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="3"/>
       <c r="D8" s="18"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickTop="1"/>
-    <row r="10" spans="1:5" ht="27" thickBot="1">
+    <row r="9" spans="1:5" ht="15" thickTop="1"/>
+    <row r="10" spans="1:5" ht="26.6" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -2395,7 +2476,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+    <row r="11" spans="1:5" ht="18.45" thickTop="1" thickBot="1">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30.75" thickTop="1" thickBot="1">
+    <row r="12" spans="1:5" ht="29.6" thickTop="1" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -2429,7 +2510,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31.5" thickTop="1" thickBot="1">
+    <row r="13" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A13" s="13" t="s">
         <v>9</v>
       </c>
@@ -2446,7 +2527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" thickTop="1" thickBot="1">
+    <row r="14" spans="1:5" ht="43.75" thickTop="1" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2463,7 +2544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.5" thickTop="1" thickBot="1">
+    <row r="15" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
@@ -2480,32 +2561,32 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="60.75" thickTop="1" thickBot="1">
+    <row r="16" spans="1:5" ht="57.45" thickTop="1" thickBot="1">
       <c r="A16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="D16" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    </row>
+    <row r="17" spans="1:5" ht="15.45" thickTop="1" thickBot="1">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="19"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickTop="1"/>
-    <row r="19" spans="1:5" ht="27" thickBot="1">
+    <row r="18" spans="1:5" ht="15" thickTop="1"/>
+    <row r="19" spans="1:5" ht="26.6" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
@@ -2514,7 +2595,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+    <row r="20" spans="1:5" ht="18.45" thickTop="1" thickBot="1">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -2531,7 +2612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="21" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A21" s="14" t="s">
         <v>38</v>
       </c>
@@ -2548,7 +2629,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="22" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A22" s="15" t="s">
         <v>40</v>
       </c>
@@ -2565,7 +2646,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="23" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A23" s="14" t="s">
         <v>41</v>
       </c>
@@ -2582,15 +2663,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    <row r="24" spans="1:5" ht="15.45" thickTop="1" thickBot="1">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="19"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickTop="1"/>
-    <row r="26" spans="1:5" ht="27" thickBot="1">
+    <row r="25" spans="1:5" ht="15" thickTop="1"/>
+    <row r="26" spans="1:5" ht="26.6" thickBot="1">
       <c r="A26" s="6" t="s">
         <v>49</v>
       </c>
@@ -2599,7 +2680,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+    <row r="27" spans="1:5" ht="18.45" thickTop="1" thickBot="1">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -2616,7 +2697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="28" spans="1:5" ht="26.6" thickTop="1" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
@@ -2631,7 +2712,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="29" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A29" s="13" t="s">
         <v>52</v>
       </c>
@@ -2648,7 +2729,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" thickTop="1" thickBot="1">
+    <row r="30" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A30" s="16" t="s">
         <v>55</v>
       </c>
@@ -2699,15 +2780,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    <row r="33" spans="1:5" ht="15.45" thickTop="1" thickBot="1">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="19"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickTop="1"/>
-    <row r="35" spans="1:5" ht="27" thickBot="1">
+    <row r="34" spans="1:5" ht="15" thickTop="1"/>
+    <row r="35" spans="1:5" ht="26.6" thickBot="1">
       <c r="A35" s="6" t="s">
         <v>69</v>
       </c>
@@ -2716,7 +2797,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" ht="19.5" thickTop="1" thickBot="1">
+    <row r="36" spans="1:5" ht="18.45" thickTop="1" thickBot="1">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2733,12 +2814,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="59.25" thickTop="1" thickBot="1">
+    <row r="37" spans="1:5" ht="57.45" thickTop="1" thickBot="1">
       <c r="A37" s="13" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>71</v>
@@ -2747,7 +2828,7 @@
         <v>8</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="66.75" customHeight="1" thickTop="1" thickBot="1">
@@ -2755,7 +2836,7 @@
         <v>72</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>71</v>
@@ -2764,7 +2845,7 @@
         <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
@@ -2772,7 +2853,7 @@
         <v>73</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>74</v>
@@ -2781,7 +2862,7 @@
         <v>8</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
@@ -2789,16 +2870,16 @@
         <v>75</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="73.5" customHeight="1" thickTop="1" thickBot="1">
@@ -2806,7 +2887,7 @@
         <v>77</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>76</v>
@@ -2815,32 +2896,32 @@
         <v>8</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="104.25" customHeight="1" thickTop="1" thickBot="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="147" customHeight="1" thickTop="1" thickBot="1">
       <c r="A42" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A43" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>32</v>
@@ -2852,10 +2933,10 @@
     </row>
     <row r="44" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A44" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>39</v>
@@ -2864,15 +2945,15 @@
         <v>2</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A45" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>39</v>
@@ -2881,15 +2962,15 @@
         <v>5</v>
       </c>
       <c r="E45" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
+      <c r="A46" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="30.75" thickTop="1" thickBot="1">
-      <c r="A46" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>39</v>
@@ -2898,15 +2979,15 @@
         <v>10</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="30.75" thickTop="1" thickBot="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A47" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>39</v>
@@ -2915,15 +2996,15 @@
         <v>2</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="45" thickTop="1" thickBot="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="43.3" thickTop="1" thickBot="1">
       <c r="A48" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>39</v>
@@ -2932,15 +3013,15 @@
         <v>2</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" thickTop="1" thickBot="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="29.15" thickTop="1" thickBot="1">
       <c r="A49" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>32</v>
@@ -2950,32 +3031,33 @@
       </c>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="45.75" thickTop="1" thickBot="1">
+    <row r="50" spans="1:5" ht="43.3" thickTop="1" thickBot="1">
       <c r="A50" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    </row>
+    <row r="51" spans="1:5" ht="15.45" thickTop="1" thickBot="1">
       <c r="A51" s="17"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="29"/>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" thickTop="1"/>
+    <row r="52" spans="1:5" ht="15" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>